<commit_message>
FIX: Test also full rows and columns in IRR function
This means functions like `=IRR(A:A)` or `=IRR(1:1)`
</commit_message>
<xml_diff>
--- a/xlsx/tests/calc_tests/IRR.xlsx
+++ b/xlsx/tests/calc_tests/IRR.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC2A0B81-E134-8B40-8F1A-A3317686D08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{158F2EBB-11CC-40EA-ABFF-0329936C936B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{A0705745-E7DF-B343-9A23-E8010C92D60D}"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" firstSheet="3" activeTab="4" xr2:uid="{A0705745-E7DF-B343-9A23-E8010C92D60D}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="Two Values" sheetId="2" r:id="rId2"/>
     <sheet name="Three Parameters" sheetId="3" r:id="rId3"/>
-    <sheet name="METADATA" sheetId="4" r:id="rId4"/>
+    <sheet name="FullRow" sheetId="5" r:id="rId4"/>
+    <sheet name="FullColumn" sheetId="6" r:id="rId5"/>
+    <sheet name="METADATA" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,9 +52,6 @@
     <t>value 3</t>
   </si>
   <si>
-    <t>guess</t>
-  </si>
-  <si>
     <t>value 4</t>
   </si>
   <si>
@@ -62,16 +61,25 @@
     <t>value 6</t>
   </si>
   <si>
-    <t>NPV</t>
+    <t>guess</t>
   </si>
   <si>
     <t>IRR</t>
   </si>
   <si>
+    <t>NPV</t>
+  </si>
+  <si>
+    <t>One single argument produces #NUM!</t>
+  </si>
+  <si>
     <t>Hello</t>
   </si>
   <si>
-    <t>One single argument produces #NUM!</t>
+    <t>&lt;= empty spaces are not like 0's</t>
+  </si>
+  <si>
+    <t>&lt;= trivial cero</t>
   </si>
   <si>
     <t>v0</t>
@@ -83,19 +91,13 @@
     <t>-V1/v0 - 1</t>
   </si>
   <si>
-    <t>v2</t>
-  </si>
-  <si>
     <t>Two variables is exactly solvable</t>
   </si>
   <si>
     <t>&lt;= Although there is a solution, the function is not defined for all positive or negative values</t>
   </si>
   <si>
-    <t>&lt;= empty spaces are not like 0's</t>
-  </si>
-  <si>
-    <t>&lt;= trivial cero</t>
+    <t>v2</t>
   </si>
 </sst>
 </file>
@@ -103,9 +105,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,14 +201,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -527,15 +529,15 @@
   <dimension ref="A1:R59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
     <col min="12" max="12" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -546,25 +548,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="L1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>-20</v>
       </c>
@@ -603,10 +605,10 @@
         <v>#NUM!</v>
       </c>
       <c r="R2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>-1000</v>
       </c>
@@ -645,7 +647,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>-55</v>
       </c>
@@ -684,7 +686,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>-20</v>
       </c>
@@ -716,7 +718,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>20</v>
       </c>
@@ -736,7 +738,7 @@
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" si="0"/>
@@ -751,7 +753,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>20</v>
       </c>
@@ -783,7 +785,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>-70</v>
       </c>
@@ -809,7 +811,7 @@
         <v>-0.44350694133493618</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>-20</v>
       </c>
@@ -844,7 +846,7 @@
         <v>0.14866576379560037</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>-20</v>
       </c>
@@ -873,7 +875,7 @@
       </c>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>-20</v>
       </c>
@@ -902,7 +904,7 @@
       </c>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>-20</v>
       </c>
@@ -931,7 +933,7 @@
       </c>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>-20</v>
       </c>
@@ -960,7 +962,7 @@
       </c>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>20</v>
       </c>
@@ -989,7 +991,7 @@
       </c>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>-1</v>
       </c>
@@ -1018,7 +1020,7 @@
       </c>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>40</v>
       </c>
@@ -1047,7 +1049,7 @@
       </c>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14">
       <c r="A17">
         <v>-400</v>
       </c>
@@ -1076,7 +1078,7 @@
       </c>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14">
       <c r="A18">
         <v>-30</v>
       </c>
@@ -1105,7 +1107,7 @@
       </c>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14">
       <c r="A19">
         <v>-20</v>
       </c>
@@ -1113,7 +1115,7 @@
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -1133,7 +1135,7 @@
         <v>-8.5990125592647461E-14</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14">
       <c r="A20">
         <v>-20</v>
       </c>
@@ -1147,14 +1149,14 @@
         <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="L20" s="2">
         <f t="shared" si="0"/>
         <v>-7.3008438340145698E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14">
       <c r="A21">
         <v>-20</v>
       </c>
@@ -1178,7 +1180,7 @@
         <v>-5.230275377659388E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14">
       <c r="A22">
         <v>-130</v>
       </c>
@@ -1198,14 +1200,14 @@
         <v>30</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="L22" s="2">
         <f t="shared" si="0"/>
         <v>2.4507063045575705E-12</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14">
       <c r="A23">
         <v>-20</v>
       </c>
@@ -1223,7 +1225,7 @@
         <v>-7.3008438340145698E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="A24">
         <v>-20</v>
       </c>
@@ -1247,7 +1249,7 @@
         <v>-7.3008438340145698E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14">
       <c r="A25">
         <v>-100</v>
       </c>
@@ -1271,7 +1273,7 @@
         <v>9.4591675366124672E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14">
       <c r="A26">
         <v>-125</v>
       </c>
@@ -1295,7 +1297,7 @@
         <v>1.3222156208353208E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14">
       <c r="A27">
         <v>-120</v>
       </c>
@@ -1323,7 +1325,7 @@
         <v>2.7307616095139098E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14">
       <c r="A28">
         <v>-115</v>
       </c>
@@ -1347,7 +1349,7 @@
         <v>4.2357506565785519E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14">
       <c r="A29">
         <v>-110</v>
       </c>
@@ -1371,7 +1373,7 @@
         <v>5.8490370511013801E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14">
       <c r="A30">
         <v>-105</v>
       </c>
@@ -1395,7 +1397,7 @@
         <v>7.5846201635883181E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14">
       <c r="A31">
         <v>-100</v>
       </c>
@@ -1419,7 +1421,7 @@
         <v>9.4591675366124672E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14">
       <c r="A32">
         <v>-95</v>
       </c>
@@ -1443,7 +1445,7 @@
         <v>0.11492701537265648</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>-90</v>
       </c>
@@ -1467,7 +1469,7 @@
         <v>0.13709513129836592</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>-85</v>
       </c>
@@ -1491,7 +1493,7 @@
         <v>0.16139396386165483</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>-80</v>
       </c>
@@ -1515,7 +1517,7 @@
         <v>0.18819344430894169</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>-75</v>
       </c>
@@ -1539,7 +1541,7 @@
         <v>0.21795923201880574</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>-70</v>
       </c>
@@ -1563,7 +1565,7 @@
         <v>0.25128664113527588</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>-65</v>
       </c>
@@ -1587,7 +1589,7 @@
         <v>0.2889502891732405</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>-60</v>
       </c>
@@ -1611,7 +1613,7 @@
         <v>0.33197873322992688</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>-55</v>
       </c>
@@ -1635,7 +1637,7 @@
         <v>0.38177018762394832</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>-50</v>
       </c>
@@ -1659,7 +1661,7 @@
         <v>0.44027847722734781</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>-45</v>
       </c>
@@ -1683,7 +1685,7 @@
         <v>0.5103246911340793</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>-40</v>
       </c>
@@ -1707,7 +1709,7 @@
         <v>0.59614634175645853</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>-35</v>
       </c>
@@ -1731,7 +1733,7 @@
         <v>0.70442563609490527</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>-30</v>
       </c>
@@ -1755,7 +1757,7 @@
         <v>0.84636551362651602</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>-25</v>
       </c>
@@ -1779,7 +1781,7 @@
         <v>1.0423044576428886</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>-20</v>
       </c>
@@ -1803,7 +1805,7 @@
         <v>1.3333765085060993</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>-135</v>
       </c>
@@ -1827,7 +1829,7 @@
         <v>-1.2445711327526809E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12">
       <c r="A49">
         <v>-140</v>
       </c>
@@ -1851,7 +1853,7 @@
         <v>-2.4190050166356225E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12">
       <c r="A50">
         <v>-145</v>
       </c>
@@ -1875,7 +1877,7 @@
         <v>-3.529827791690443E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12">
       <c r="A51">
         <v>-150</v>
       </c>
@@ -1899,7 +1901,7 @@
         <v>-4.5827431442258204E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12">
       <c r="A52">
         <v>-155</v>
       </c>
@@ -1923,7 +1925,7 @@
         <v>-5.5827607681748326E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12">
       <c r="A53">
         <v>-160</v>
       </c>
@@ -1947,7 +1949,7 @@
         <v>-6.5343011839821386E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12">
       <c r="A54">
         <v>-165</v>
       </c>
@@ -1971,7 +1973,7 @@
         <v>-7.4412818777553347E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12">
       <c r="A55">
         <v>-170</v>
       </c>
@@ -1995,7 +1997,7 @@
         <v>-8.3071885619666275E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12">
       <c r="A56">
         <v>-175</v>
       </c>
@@ -2019,7 +2021,7 @@
         <v>-9.1351344955906466E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12">
       <c r="A57">
         <v>-180</v>
       </c>
@@ -2043,7 +2045,7 @@
         <v>-9.9279101534061387E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12">
       <c r="A58">
         <v>-185</v>
       </c>
@@ -2067,7 +2069,7 @@
         <v>-0.10688025044042104</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12">
       <c r="A59">
         <v>-190</v>
       </c>
@@ -2104,23 +2106,23 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>-2</v>
       </c>
@@ -2136,10 +2138,10 @@
         <v>1.5</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2155,10 +2157,10 @@
         <v>-3</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>-4</v>
       </c>
@@ -2174,7 +2176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2190,7 +2192,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>-5</v>
       </c>
@@ -2206,7 +2208,7 @@
         <v>-0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>-2</v>
       </c>
@@ -2222,7 +2224,7 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2238,7 +2240,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>-2</v>
       </c>
@@ -2254,7 +2256,7 @@
         <v>-2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -2270,7 +2272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2286,7 +2288,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="C12" s="1"/>
     </row>
   </sheetData>
@@ -2302,26 +2304,26 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2340,7 +2342,7 @@
         <v>1.187938506697367E-14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2359,7 +2361,7 @@
         <v>2.5054956076341091E-14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>-1</v>
       </c>
@@ -2378,7 +2380,7 @@
         <v>9.1912870455508683E-16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>-3</v>
       </c>
@@ -2403,16 +2405,218 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E335226C-2C77-4993-8D8C-9A4433642861}">
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1">
+        <v>-2</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>-4</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>2</v>
+      </c>
+      <c r="N1" s="2">
+        <f>IRR(A:A)</f>
+        <v>1.5</v>
+      </c>
+      <c r="O1" s="2" t="e">
+        <f>IRR(B:B)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P1" s="2">
+        <f>IRR(C:C)</f>
+        <v>0</v>
+      </c>
+      <c r="Q1" s="2">
+        <f>IRR(D:D)</f>
+        <v>1.0913995107664221E-7</v>
+      </c>
+      <c r="R1" s="2">
+        <f>IRR(E:E)</f>
+        <v>-0.14921894064178554</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>-2</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2">
+        <f>NPV(N1, A:A)</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="2" t="e">
+        <f t="shared" ref="O2:R2" si="0">NPV(O1, B:B)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="P2" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2">
+        <f t="shared" si="0"/>
+        <v>1.187938506697367E-14</v>
+      </c>
+      <c r="R2" s="2">
+        <f t="shared" si="0"/>
+        <v>2.5054956076341091E-14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA4C9E6-70F0-447C-BECA-2E2C206E7B9F}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1">
+        <v>-20</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>5</v>
+      </c>
+      <c r="D1">
+        <v>5</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>-1000</v>
+      </c>
+      <c r="B2">
+        <v>230</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2">
+        <v>125</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>-55</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2">
+        <f>IRR(1:1)</f>
+        <v>7.9308261160397242E-2</v>
+      </c>
+      <c r="B21" s="2">
+        <f>NPV(A21,1:1)</f>
+        <v>6.4212018552224666E-12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2">
+        <f t="shared" ref="A22:A23" si="0">IRR(2:2)</f>
+        <v>-0.1015006760535847</v>
+      </c>
+      <c r="B22" s="2">
+        <f t="shared" ref="B22:B23" si="1">NPV(A22,2:2)</f>
+        <v>-2.8358465972398184E-11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2">
+        <f t="shared" si="0"/>
+        <v>-0.1884564442514256</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" si="1"/>
+        <v>6.080439711727234E-11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A86C73E-B491-D14F-95E3-0838E2BC1E45}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="11">
         <v>4.9999999999999998E-7</v>
       </c>

</xml_diff>